<commit_message>
updated files to be uniform
</commit_message>
<xml_diff>
--- a/bioSample/bioSample_hbrown_01.16.20.xlsx
+++ b/bioSample/bioSample_hbrown_01.16.20.xlsx
@@ -1,14 +1,14 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10908"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10308"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/hollybrown/Library/Containers/com.microsoft.Excel/Data/Desktop/6a metadata sheets/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/hollybrown/database_files/bioSample/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{13E8D547-A09E-8E49-A25F-651CE1BAFD39}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{F3A347DF-6060-CE4B-BE88-1416E0200A6D}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="13560" yWindow="460" windowWidth="20040" windowHeight="18940" xr2:uid="{F6F00F34-BB7B-AE4F-B1EE-64EE76BE41DA}"/>
   </bookViews>
@@ -68,9 +68,6 @@
     <t>harvestDate</t>
   </si>
   <si>
-    <t>BROWN</t>
-  </si>
-  <si>
     <t>CNAG_00000</t>
   </si>
   <si>
@@ -105,6 +102,9 @@
   </si>
   <si>
     <t>01.16.20</t>
+  </si>
+  <si>
+    <t>H.BROWN</t>
   </si>
 </sst>
 </file>
@@ -482,7 +482,7 @@
   <dimension ref="A1:Z27"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="A3" sqref="A3:A27"/>
+      <selection activeCell="B3" sqref="B3:B27"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -545,31 +545,31 @@
     </row>
     <row r="2" spans="1:26" x14ac:dyDescent="0.2">
       <c r="A2" t="s">
-        <v>24</v>
+        <v>23</v>
       </c>
       <c r="B2" t="s">
-        <v>12</v>
+        <v>24</v>
       </c>
       <c r="C2">
         <v>1</v>
       </c>
       <c r="D2" s="2" t="s">
-        <v>15</v>
+        <v>14</v>
       </c>
       <c r="F2" t="s">
-        <v>17</v>
+        <v>16</v>
       </c>
       <c r="G2" t="s">
+        <v>12</v>
+      </c>
+      <c r="H2" s="1" t="s">
+        <v>15</v>
+      </c>
+      <c r="I2" s="3" t="s">
+        <v>15</v>
+      </c>
+      <c r="J2" t="s">
         <v>13</v>
-      </c>
-      <c r="H2" s="1" t="s">
-        <v>16</v>
-      </c>
-      <c r="I2" s="3" t="s">
-        <v>16</v>
-      </c>
-      <c r="J2" t="s">
-        <v>14</v>
       </c>
       <c r="K2">
         <v>0</v>
@@ -593,31 +593,31 @@
     </row>
     <row r="3" spans="1:26" x14ac:dyDescent="0.2">
       <c r="A3" t="s">
-        <v>24</v>
+        <v>23</v>
       </c>
       <c r="B3" t="s">
-        <v>12</v>
+        <v>24</v>
       </c>
       <c r="C3">
         <v>2</v>
       </c>
       <c r="D3" s="2" t="s">
-        <v>15</v>
+        <v>14</v>
       </c>
       <c r="F3" t="s">
-        <v>17</v>
+        <v>16</v>
       </c>
       <c r="G3" t="s">
+        <v>12</v>
+      </c>
+      <c r="H3" s="1" t="s">
+        <v>15</v>
+      </c>
+      <c r="I3" s="3" t="s">
+        <v>15</v>
+      </c>
+      <c r="J3" t="s">
         <v>13</v>
-      </c>
-      <c r="H3" s="1" t="s">
-        <v>16</v>
-      </c>
-      <c r="I3" s="3" t="s">
-        <v>16</v>
-      </c>
-      <c r="J3" t="s">
-        <v>14</v>
       </c>
       <c r="K3">
         <v>0</v>
@@ -628,31 +628,31 @@
     </row>
     <row r="4" spans="1:26" x14ac:dyDescent="0.2">
       <c r="A4" t="s">
-        <v>24</v>
+        <v>23</v>
       </c>
       <c r="B4" t="s">
-        <v>12</v>
+        <v>24</v>
       </c>
       <c r="C4">
         <v>3</v>
       </c>
       <c r="D4" s="2" t="s">
-        <v>15</v>
+        <v>14</v>
       </c>
       <c r="F4" t="s">
+        <v>16</v>
+      </c>
+      <c r="G4" t="s">
+        <v>12</v>
+      </c>
+      <c r="H4" s="1" t="s">
+        <v>15</v>
+      </c>
+      <c r="I4" s="3" t="s">
+        <v>15</v>
+      </c>
+      <c r="J4" t="s">
         <v>17</v>
-      </c>
-      <c r="G4" t="s">
-        <v>13</v>
-      </c>
-      <c r="H4" s="1" t="s">
-        <v>16</v>
-      </c>
-      <c r="I4" s="3" t="s">
-        <v>16</v>
-      </c>
-      <c r="J4" t="s">
-        <v>18</v>
       </c>
       <c r="K4">
         <v>30</v>
@@ -663,31 +663,31 @@
     </row>
     <row r="5" spans="1:26" x14ac:dyDescent="0.2">
       <c r="A5" t="s">
-        <v>24</v>
+        <v>23</v>
       </c>
       <c r="B5" t="s">
-        <v>12</v>
+        <v>24</v>
       </c>
       <c r="C5">
         <v>4</v>
       </c>
       <c r="D5" s="2" t="s">
-        <v>15</v>
+        <v>14</v>
       </c>
       <c r="F5" t="s">
-        <v>17</v>
+        <v>16</v>
       </c>
       <c r="G5" t="s">
-        <v>13</v>
+        <v>12</v>
       </c>
       <c r="H5" s="1" t="s">
-        <v>16</v>
+        <v>15</v>
       </c>
       <c r="I5" s="3" t="s">
-        <v>16</v>
+        <v>15</v>
       </c>
       <c r="J5" t="s">
-        <v>19</v>
+        <v>18</v>
       </c>
       <c r="K5">
         <v>30</v>
@@ -698,31 +698,31 @@
     </row>
     <row r="6" spans="1:26" x14ac:dyDescent="0.2">
       <c r="A6" t="s">
-        <v>24</v>
+        <v>23</v>
       </c>
       <c r="B6" t="s">
-        <v>12</v>
+        <v>24</v>
       </c>
       <c r="C6">
         <v>5</v>
       </c>
       <c r="D6" s="2" t="s">
-        <v>15</v>
+        <v>14</v>
       </c>
       <c r="F6" t="s">
-        <v>17</v>
+        <v>16</v>
       </c>
       <c r="G6" t="s">
-        <v>13</v>
+        <v>12</v>
       </c>
       <c r="H6" s="1" t="s">
-        <v>16</v>
+        <v>15</v>
       </c>
       <c r="I6" s="3" t="s">
-        <v>16</v>
+        <v>15</v>
       </c>
       <c r="J6" t="s">
-        <v>20</v>
+        <v>19</v>
       </c>
       <c r="K6">
         <v>30</v>
@@ -733,31 +733,31 @@
     </row>
     <row r="7" spans="1:26" x14ac:dyDescent="0.2">
       <c r="A7" t="s">
-        <v>24</v>
+        <v>23</v>
       </c>
       <c r="B7" t="s">
-        <v>12</v>
+        <v>24</v>
       </c>
       <c r="C7">
         <v>6</v>
       </c>
       <c r="D7" s="2" t="s">
-        <v>15</v>
+        <v>14</v>
       </c>
       <c r="F7" t="s">
-        <v>17</v>
+        <v>16</v>
       </c>
       <c r="G7" t="s">
-        <v>13</v>
+        <v>12</v>
       </c>
       <c r="H7" s="1" t="s">
-        <v>16</v>
+        <v>15</v>
       </c>
       <c r="I7" s="3" t="s">
-        <v>16</v>
+        <v>15</v>
       </c>
       <c r="J7" t="s">
-        <v>21</v>
+        <v>20</v>
       </c>
       <c r="K7">
         <v>30</v>
@@ -768,31 +768,31 @@
     </row>
     <row r="8" spans="1:26" x14ac:dyDescent="0.2">
       <c r="A8" t="s">
-        <v>24</v>
+        <v>23</v>
       </c>
       <c r="B8" t="s">
-        <v>12</v>
+        <v>24</v>
       </c>
       <c r="C8">
         <v>7</v>
       </c>
       <c r="D8" s="2" t="s">
-        <v>15</v>
+        <v>14</v>
       </c>
       <c r="F8" t="s">
-        <v>17</v>
+        <v>16</v>
       </c>
       <c r="G8" t="s">
-        <v>13</v>
+        <v>12</v>
       </c>
       <c r="H8" s="1" t="s">
-        <v>16</v>
+        <v>15</v>
       </c>
       <c r="I8" s="3" t="s">
-        <v>16</v>
+        <v>15</v>
       </c>
       <c r="J8" t="s">
-        <v>22</v>
+        <v>21</v>
       </c>
       <c r="K8">
         <v>30</v>
@@ -803,31 +803,31 @@
     </row>
     <row r="9" spans="1:26" x14ac:dyDescent="0.2">
       <c r="A9" t="s">
-        <v>24</v>
+        <v>23</v>
       </c>
       <c r="B9" t="s">
-        <v>12</v>
+        <v>24</v>
       </c>
       <c r="C9">
         <v>8</v>
       </c>
       <c r="D9" s="2" t="s">
-        <v>15</v>
+        <v>14</v>
       </c>
       <c r="F9" t="s">
-        <v>17</v>
+        <v>16</v>
       </c>
       <c r="G9" t="s">
-        <v>13</v>
+        <v>12</v>
       </c>
       <c r="H9" s="1" t="s">
-        <v>16</v>
+        <v>15</v>
       </c>
       <c r="I9" s="3" t="s">
-        <v>16</v>
+        <v>15</v>
       </c>
       <c r="J9" t="s">
-        <v>23</v>
+        <v>22</v>
       </c>
       <c r="K9">
         <v>30</v>
@@ -838,31 +838,31 @@
     </row>
     <row r="10" spans="1:26" x14ac:dyDescent="0.2">
       <c r="A10" t="s">
-        <v>24</v>
+        <v>23</v>
       </c>
       <c r="B10" t="s">
-        <v>12</v>
+        <v>24</v>
       </c>
       <c r="C10">
         <v>9</v>
       </c>
       <c r="D10" s="2" t="s">
-        <v>15</v>
+        <v>14</v>
       </c>
       <c r="F10" t="s">
+        <v>16</v>
+      </c>
+      <c r="G10" t="s">
+        <v>12</v>
+      </c>
+      <c r="H10" s="1" t="s">
+        <v>15</v>
+      </c>
+      <c r="I10" s="3" t="s">
+        <v>15</v>
+      </c>
+      <c r="J10" t="s">
         <v>17</v>
-      </c>
-      <c r="G10" t="s">
-        <v>13</v>
-      </c>
-      <c r="H10" s="1" t="s">
-        <v>16</v>
-      </c>
-      <c r="I10" s="3" t="s">
-        <v>16</v>
-      </c>
-      <c r="J10" t="s">
-        <v>18</v>
       </c>
       <c r="K10">
         <v>90</v>
@@ -873,31 +873,31 @@
     </row>
     <row r="11" spans="1:26" x14ac:dyDescent="0.2">
       <c r="A11" t="s">
-        <v>24</v>
+        <v>23</v>
       </c>
       <c r="B11" t="s">
-        <v>12</v>
+        <v>24</v>
       </c>
       <c r="C11">
         <v>10</v>
       </c>
       <c r="D11" s="2" t="s">
-        <v>15</v>
+        <v>14</v>
       </c>
       <c r="F11" t="s">
-        <v>17</v>
+        <v>16</v>
       </c>
       <c r="G11" t="s">
-        <v>13</v>
+        <v>12</v>
       </c>
       <c r="H11" s="1" t="s">
-        <v>16</v>
+        <v>15</v>
       </c>
       <c r="I11" s="3" t="s">
-        <v>16</v>
+        <v>15</v>
       </c>
       <c r="J11" t="s">
-        <v>19</v>
+        <v>18</v>
       </c>
       <c r="K11">
         <v>90</v>
@@ -908,31 +908,31 @@
     </row>
     <row r="12" spans="1:26" x14ac:dyDescent="0.2">
       <c r="A12" t="s">
-        <v>24</v>
+        <v>23</v>
       </c>
       <c r="B12" t="s">
-        <v>12</v>
+        <v>24</v>
       </c>
       <c r="C12">
         <v>11</v>
       </c>
       <c r="D12" s="2" t="s">
-        <v>15</v>
+        <v>14</v>
       </c>
       <c r="F12" t="s">
-        <v>17</v>
+        <v>16</v>
       </c>
       <c r="G12" t="s">
-        <v>13</v>
+        <v>12</v>
       </c>
       <c r="H12" s="1" t="s">
-        <v>16</v>
+        <v>15</v>
       </c>
       <c r="I12" s="3" t="s">
-        <v>16</v>
+        <v>15</v>
       </c>
       <c r="J12" t="s">
-        <v>20</v>
+        <v>19</v>
       </c>
       <c r="K12">
         <v>90</v>
@@ -943,31 +943,31 @@
     </row>
     <row r="13" spans="1:26" x14ac:dyDescent="0.2">
       <c r="A13" t="s">
-        <v>24</v>
+        <v>23</v>
       </c>
       <c r="B13" t="s">
-        <v>12</v>
+        <v>24</v>
       </c>
       <c r="C13">
         <v>12</v>
       </c>
       <c r="D13" s="2" t="s">
-        <v>15</v>
+        <v>14</v>
       </c>
       <c r="F13" t="s">
-        <v>17</v>
+        <v>16</v>
       </c>
       <c r="G13" t="s">
-        <v>13</v>
+        <v>12</v>
       </c>
       <c r="H13" s="1" t="s">
-        <v>16</v>
+        <v>15</v>
       </c>
       <c r="I13" s="3" t="s">
-        <v>16</v>
+        <v>15</v>
       </c>
       <c r="J13" t="s">
-        <v>21</v>
+        <v>20</v>
       </c>
       <c r="K13">
         <v>90</v>
@@ -978,31 +978,31 @@
     </row>
     <row r="14" spans="1:26" x14ac:dyDescent="0.2">
       <c r="A14" t="s">
-        <v>24</v>
+        <v>23</v>
       </c>
       <c r="B14" t="s">
-        <v>12</v>
+        <v>24</v>
       </c>
       <c r="C14">
         <v>13</v>
       </c>
       <c r="D14" s="2" t="s">
-        <v>15</v>
+        <v>14</v>
       </c>
       <c r="F14" t="s">
-        <v>17</v>
+        <v>16</v>
       </c>
       <c r="G14" t="s">
-        <v>13</v>
+        <v>12</v>
       </c>
       <c r="H14" s="1" t="s">
-        <v>16</v>
+        <v>15</v>
       </c>
       <c r="I14" s="3" t="s">
-        <v>16</v>
+        <v>15</v>
       </c>
       <c r="J14" t="s">
-        <v>22</v>
+        <v>21</v>
       </c>
       <c r="K14">
         <v>90</v>
@@ -1013,31 +1013,31 @@
     </row>
     <row r="15" spans="1:26" x14ac:dyDescent="0.2">
       <c r="A15" t="s">
-        <v>24</v>
+        <v>23</v>
       </c>
       <c r="B15" t="s">
-        <v>12</v>
+        <v>24</v>
       </c>
       <c r="C15">
         <v>14</v>
       </c>
       <c r="D15" s="2" t="s">
-        <v>15</v>
+        <v>14</v>
       </c>
       <c r="F15" t="s">
-        <v>17</v>
+        <v>16</v>
       </c>
       <c r="G15" t="s">
-        <v>13</v>
+        <v>12</v>
       </c>
       <c r="H15" s="1" t="s">
-        <v>16</v>
+        <v>15</v>
       </c>
       <c r="I15" s="3" t="s">
-        <v>16</v>
+        <v>15</v>
       </c>
       <c r="J15" t="s">
-        <v>23</v>
+        <v>22</v>
       </c>
       <c r="K15">
         <v>90</v>
@@ -1048,31 +1048,31 @@
     </row>
     <row r="16" spans="1:26" x14ac:dyDescent="0.2">
       <c r="A16" t="s">
-        <v>24</v>
+        <v>23</v>
       </c>
       <c r="B16" t="s">
-        <v>12</v>
+        <v>24</v>
       </c>
       <c r="C16">
         <v>15</v>
       </c>
       <c r="D16" s="2" t="s">
-        <v>15</v>
+        <v>14</v>
       </c>
       <c r="F16" t="s">
+        <v>16</v>
+      </c>
+      <c r="G16" t="s">
+        <v>12</v>
+      </c>
+      <c r="H16" s="1" t="s">
+        <v>15</v>
+      </c>
+      <c r="I16" s="3" t="s">
+        <v>15</v>
+      </c>
+      <c r="J16" t="s">
         <v>17</v>
-      </c>
-      <c r="G16" t="s">
-        <v>13</v>
-      </c>
-      <c r="H16" s="1" t="s">
-        <v>16</v>
-      </c>
-      <c r="I16" s="3" t="s">
-        <v>16</v>
-      </c>
-      <c r="J16" t="s">
-        <v>18</v>
       </c>
       <c r="K16">
         <v>180</v>
@@ -1083,31 +1083,31 @@
     </row>
     <row r="17" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A17" t="s">
-        <v>24</v>
+        <v>23</v>
       </c>
       <c r="B17" t="s">
-        <v>12</v>
+        <v>24</v>
       </c>
       <c r="C17">
         <v>16</v>
       </c>
       <c r="D17" s="2" t="s">
-        <v>15</v>
+        <v>14</v>
       </c>
       <c r="F17" t="s">
-        <v>17</v>
+        <v>16</v>
       </c>
       <c r="G17" t="s">
-        <v>13</v>
+        <v>12</v>
       </c>
       <c r="H17" s="1" t="s">
-        <v>16</v>
+        <v>15</v>
       </c>
       <c r="I17" s="3" t="s">
-        <v>16</v>
+        <v>15</v>
       </c>
       <c r="J17" t="s">
-        <v>19</v>
+        <v>18</v>
       </c>
       <c r="K17">
         <v>180</v>
@@ -1118,31 +1118,31 @@
     </row>
     <row r="18" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A18" t="s">
-        <v>24</v>
+        <v>23</v>
       </c>
       <c r="B18" t="s">
-        <v>12</v>
+        <v>24</v>
       </c>
       <c r="C18">
         <v>17</v>
       </c>
       <c r="D18" s="2" t="s">
-        <v>15</v>
+        <v>14</v>
       </c>
       <c r="F18" t="s">
-        <v>17</v>
+        <v>16</v>
       </c>
       <c r="G18" t="s">
-        <v>13</v>
+        <v>12</v>
       </c>
       <c r="H18" s="1" t="s">
-        <v>16</v>
+        <v>15</v>
       </c>
       <c r="I18" s="3" t="s">
-        <v>16</v>
+        <v>15</v>
       </c>
       <c r="J18" t="s">
-        <v>20</v>
+        <v>19</v>
       </c>
       <c r="K18">
         <v>180</v>
@@ -1153,31 +1153,31 @@
     </row>
     <row r="19" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A19" t="s">
-        <v>24</v>
+        <v>23</v>
       </c>
       <c r="B19" t="s">
-        <v>12</v>
+        <v>24</v>
       </c>
       <c r="C19">
         <v>18</v>
       </c>
       <c r="D19" s="2" t="s">
-        <v>15</v>
+        <v>14</v>
       </c>
       <c r="F19" t="s">
-        <v>17</v>
+        <v>16</v>
       </c>
       <c r="G19" t="s">
-        <v>13</v>
+        <v>12</v>
       </c>
       <c r="H19" s="1" t="s">
-        <v>16</v>
+        <v>15</v>
       </c>
       <c r="I19" s="3" t="s">
-        <v>16</v>
+        <v>15</v>
       </c>
       <c r="J19" t="s">
-        <v>21</v>
+        <v>20</v>
       </c>
       <c r="K19">
         <v>180</v>
@@ -1188,31 +1188,31 @@
     </row>
     <row r="20" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A20" t="s">
-        <v>24</v>
+        <v>23</v>
       </c>
       <c r="B20" t="s">
-        <v>12</v>
+        <v>24</v>
       </c>
       <c r="C20">
         <v>19</v>
       </c>
       <c r="D20" s="2" t="s">
-        <v>15</v>
+        <v>14</v>
       </c>
       <c r="F20" t="s">
-        <v>17</v>
+        <v>16</v>
       </c>
       <c r="G20" t="s">
-        <v>13</v>
+        <v>12</v>
       </c>
       <c r="H20" s="1" t="s">
-        <v>16</v>
+        <v>15</v>
       </c>
       <c r="I20" s="3" t="s">
-        <v>16</v>
+        <v>15</v>
       </c>
       <c r="J20" t="s">
-        <v>22</v>
+        <v>21</v>
       </c>
       <c r="K20">
         <v>180</v>
@@ -1223,31 +1223,31 @@
     </row>
     <row r="21" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A21" t="s">
-        <v>24</v>
+        <v>23</v>
       </c>
       <c r="B21" t="s">
-        <v>12</v>
+        <v>24</v>
       </c>
       <c r="C21">
         <v>20</v>
       </c>
       <c r="D21" s="2" t="s">
-        <v>15</v>
+        <v>14</v>
       </c>
       <c r="F21" t="s">
-        <v>17</v>
+        <v>16</v>
       </c>
       <c r="G21" t="s">
-        <v>13</v>
+        <v>12</v>
       </c>
       <c r="H21" s="1" t="s">
-        <v>16</v>
+        <v>15</v>
       </c>
       <c r="I21" s="3" t="s">
-        <v>16</v>
+        <v>15</v>
       </c>
       <c r="J21" t="s">
-        <v>23</v>
+        <v>22</v>
       </c>
       <c r="K21">
         <v>180</v>
@@ -1258,31 +1258,31 @@
     </row>
     <row r="22" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A22" t="s">
-        <v>24</v>
+        <v>23</v>
       </c>
       <c r="B22" t="s">
-        <v>12</v>
+        <v>24</v>
       </c>
       <c r="C22">
         <v>21</v>
       </c>
       <c r="D22" s="2" t="s">
-        <v>15</v>
+        <v>14</v>
       </c>
       <c r="F22" t="s">
+        <v>16</v>
+      </c>
+      <c r="G22" t="s">
+        <v>12</v>
+      </c>
+      <c r="H22" s="1" t="s">
+        <v>15</v>
+      </c>
+      <c r="I22" s="3" t="s">
+        <v>15</v>
+      </c>
+      <c r="J22" t="s">
         <v>17</v>
-      </c>
-      <c r="G22" t="s">
-        <v>13</v>
-      </c>
-      <c r="H22" s="1" t="s">
-        <v>16</v>
-      </c>
-      <c r="I22" s="3" t="s">
-        <v>16</v>
-      </c>
-      <c r="J22" t="s">
-        <v>18</v>
       </c>
       <c r="K22">
         <v>1440</v>
@@ -1293,31 +1293,31 @@
     </row>
     <row r="23" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A23" t="s">
-        <v>24</v>
+        <v>23</v>
       </c>
       <c r="B23" t="s">
-        <v>12</v>
+        <v>24</v>
       </c>
       <c r="C23">
         <v>22</v>
       </c>
       <c r="D23" s="2" t="s">
-        <v>15</v>
+        <v>14</v>
       </c>
       <c r="F23" t="s">
-        <v>17</v>
+        <v>16</v>
       </c>
       <c r="G23" t="s">
-        <v>13</v>
+        <v>12</v>
       </c>
       <c r="H23" s="1" t="s">
-        <v>16</v>
+        <v>15</v>
       </c>
       <c r="I23" s="3" t="s">
-        <v>16</v>
+        <v>15</v>
       </c>
       <c r="J23" t="s">
-        <v>19</v>
+        <v>18</v>
       </c>
       <c r="K23">
         <v>1440</v>
@@ -1328,31 +1328,31 @@
     </row>
     <row r="24" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A24" t="s">
-        <v>24</v>
+        <v>23</v>
       </c>
       <c r="B24" t="s">
-        <v>12</v>
+        <v>24</v>
       </c>
       <c r="C24">
         <v>23</v>
       </c>
       <c r="D24" s="2" t="s">
-        <v>15</v>
+        <v>14</v>
       </c>
       <c r="F24" t="s">
-        <v>17</v>
+        <v>16</v>
       </c>
       <c r="G24" t="s">
-        <v>13</v>
+        <v>12</v>
       </c>
       <c r="H24" s="1" t="s">
-        <v>16</v>
+        <v>15</v>
       </c>
       <c r="I24" s="3" t="s">
-        <v>16</v>
+        <v>15</v>
       </c>
       <c r="J24" t="s">
-        <v>20</v>
+        <v>19</v>
       </c>
       <c r="K24">
         <v>1440</v>
@@ -1363,31 +1363,31 @@
     </row>
     <row r="25" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A25" t="s">
-        <v>24</v>
+        <v>23</v>
       </c>
       <c r="B25" t="s">
-        <v>12</v>
+        <v>24</v>
       </c>
       <c r="C25">
         <v>24</v>
       </c>
       <c r="D25" s="2" t="s">
-        <v>15</v>
+        <v>14</v>
       </c>
       <c r="F25" t="s">
-        <v>17</v>
+        <v>16</v>
       </c>
       <c r="G25" t="s">
-        <v>13</v>
+        <v>12</v>
       </c>
       <c r="H25" s="1" t="s">
-        <v>16</v>
+        <v>15</v>
       </c>
       <c r="I25" s="3" t="s">
-        <v>16</v>
+        <v>15</v>
       </c>
       <c r="J25" t="s">
-        <v>21</v>
+        <v>20</v>
       </c>
       <c r="K25">
         <v>1440</v>
@@ -1398,31 +1398,31 @@
     </row>
     <row r="26" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A26" t="s">
-        <v>24</v>
+        <v>23</v>
       </c>
       <c r="B26" t="s">
-        <v>12</v>
+        <v>24</v>
       </c>
       <c r="C26">
         <v>25</v>
       </c>
       <c r="D26" s="2" t="s">
-        <v>15</v>
+        <v>14</v>
       </c>
       <c r="F26" t="s">
-        <v>17</v>
+        <v>16</v>
       </c>
       <c r="G26" t="s">
-        <v>13</v>
+        <v>12</v>
       </c>
       <c r="H26" s="1" t="s">
-        <v>16</v>
+        <v>15</v>
       </c>
       <c r="I26" s="3" t="s">
-        <v>16</v>
+        <v>15</v>
       </c>
       <c r="J26" t="s">
-        <v>22</v>
+        <v>21</v>
       </c>
       <c r="K26">
         <v>1440</v>
@@ -1433,31 +1433,31 @@
     </row>
     <row r="27" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A27" t="s">
-        <v>24</v>
+        <v>23</v>
       </c>
       <c r="B27" t="s">
-        <v>12</v>
+        <v>24</v>
       </c>
       <c r="C27">
         <v>26</v>
       </c>
       <c r="D27" s="2" t="s">
-        <v>15</v>
+        <v>14</v>
       </c>
       <c r="F27" t="s">
-        <v>17</v>
+        <v>16</v>
       </c>
       <c r="G27" t="s">
-        <v>13</v>
+        <v>12</v>
       </c>
       <c r="H27" s="1" t="s">
-        <v>16</v>
+        <v>15</v>
       </c>
       <c r="I27" s="3" t="s">
-        <v>16</v>
+        <v>15</v>
       </c>
       <c r="J27" t="s">
-        <v>23</v>
+        <v>22</v>
       </c>
       <c r="K27">
         <v>1440</v>

</xml_diff>

<commit_message>
major accuracy check update
</commit_message>
<xml_diff>
--- a/bioSample/bioSample_hbrown_01.16.20.xlsx
+++ b/bioSample/bioSample_hbrown_01.16.20.xlsx
@@ -20,7 +20,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="220" uniqueCount="26">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="220" uniqueCount="25">
   <si>
     <t xml:space="preserve">harvestDate</t>
   </si>
@@ -77,9 +77,6 @@
   </si>
   <si>
     <t xml:space="preserve">PBS</t>
-  </si>
-  <si>
-    <t xml:space="preserve">biosampleNumber</t>
   </si>
   <si>
     <t xml:space="preserve">DMEM.30C.CO2.pH7</t>
@@ -107,7 +104,7 @@
   <numFmts count="1">
     <numFmt numFmtId="164" formatCode="General"/>
   </numFmts>
-  <fonts count="6">
+  <fonts count="5">
     <font>
       <sz val="12"/>
       <color rgb="FF000000"/>
@@ -129,12 +126,6 @@
       <sz val="10"/>
       <name val="Arial"/>
       <family val="0"/>
-    </font>
-    <font>
-      <sz val="12"/>
-      <color rgb="FF000000"/>
-      <name val="Calibri"/>
-      <family val="2"/>
     </font>
     <font>
       <sz val="10"/>
@@ -191,15 +182,15 @@
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false">
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
     <xf numFmtId="164" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="164" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false">
-      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
-      <protection locked="true" hidden="false"/>
-    </xf>
-    <xf numFmtId="164" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
+    <xf numFmtId="164" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
       <alignment horizontal="right" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
@@ -223,7 +214,7 @@
   <dimension ref="A1:Z27"/>
   <sheetViews>
     <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="C1" activeCellId="0" sqref="C1"/>
+      <selection pane="topLeft" activeCell="B4" activeCellId="0" sqref="B4"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="16" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
@@ -335,12 +326,12 @@
       <c r="Y2" s="2"/>
       <c r="Z2" s="2"/>
     </row>
-    <row r="3" customFormat="false" ht="16" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="3" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A3" s="0" t="s">
         <v>12</v>
       </c>
       <c r="B3" s="0" t="s">
-        <v>19</v>
+        <v>13</v>
       </c>
       <c r="C3" s="0" t="n">
         <v>2</v>
@@ -396,7 +387,7 @@
         <v>17</v>
       </c>
       <c r="J4" s="0" t="s">
-        <v>20</v>
+        <v>19</v>
       </c>
       <c r="K4" s="0" t="n">
         <v>30</v>
@@ -431,7 +422,7 @@
         <v>17</v>
       </c>
       <c r="J5" s="0" t="s">
-        <v>21</v>
+        <v>20</v>
       </c>
       <c r="K5" s="0" t="n">
         <v>30</v>
@@ -466,7 +457,7 @@
         <v>17</v>
       </c>
       <c r="J6" s="0" t="s">
-        <v>22</v>
+        <v>21</v>
       </c>
       <c r="K6" s="0" t="n">
         <v>30</v>
@@ -501,7 +492,7 @@
         <v>17</v>
       </c>
       <c r="J7" s="0" t="s">
-        <v>23</v>
+        <v>22</v>
       </c>
       <c r="K7" s="0" t="n">
         <v>30</v>
@@ -536,7 +527,7 @@
         <v>17</v>
       </c>
       <c r="J8" s="0" t="s">
-        <v>24</v>
+        <v>23</v>
       </c>
       <c r="K8" s="0" t="n">
         <v>30</v>
@@ -571,7 +562,7 @@
         <v>17</v>
       </c>
       <c r="J9" s="0" t="s">
-        <v>25</v>
+        <v>24</v>
       </c>
       <c r="K9" s="0" t="n">
         <v>30</v>
@@ -606,7 +597,7 @@
         <v>17</v>
       </c>
       <c r="J10" s="0" t="s">
-        <v>20</v>
+        <v>19</v>
       </c>
       <c r="K10" s="0" t="n">
         <v>90</v>
@@ -641,7 +632,7 @@
         <v>17</v>
       </c>
       <c r="J11" s="0" t="s">
-        <v>21</v>
+        <v>20</v>
       </c>
       <c r="K11" s="0" t="n">
         <v>90</v>
@@ -676,7 +667,7 @@
         <v>17</v>
       </c>
       <c r="J12" s="0" t="s">
-        <v>22</v>
+        <v>21</v>
       </c>
       <c r="K12" s="0" t="n">
         <v>90</v>
@@ -711,7 +702,7 @@
         <v>17</v>
       </c>
       <c r="J13" s="0" t="s">
-        <v>23</v>
+        <v>22</v>
       </c>
       <c r="K13" s="0" t="n">
         <v>90</v>
@@ -746,7 +737,7 @@
         <v>17</v>
       </c>
       <c r="J14" s="0" t="s">
-        <v>24</v>
+        <v>23</v>
       </c>
       <c r="K14" s="0" t="n">
         <v>90</v>
@@ -781,7 +772,7 @@
         <v>17</v>
       </c>
       <c r="J15" s="0" t="s">
-        <v>25</v>
+        <v>24</v>
       </c>
       <c r="K15" s="0" t="n">
         <v>90</v>
@@ -816,7 +807,7 @@
         <v>17</v>
       </c>
       <c r="J16" s="0" t="s">
-        <v>20</v>
+        <v>19</v>
       </c>
       <c r="K16" s="0" t="n">
         <v>180</v>
@@ -851,7 +842,7 @@
         <v>17</v>
       </c>
       <c r="J17" s="0" t="s">
-        <v>21</v>
+        <v>20</v>
       </c>
       <c r="K17" s="0" t="n">
         <v>180</v>
@@ -886,7 +877,7 @@
         <v>17</v>
       </c>
       <c r="J18" s="0" t="s">
-        <v>22</v>
+        <v>21</v>
       </c>
       <c r="K18" s="0" t="n">
         <v>180</v>
@@ -921,7 +912,7 @@
         <v>17</v>
       </c>
       <c r="J19" s="0" t="s">
-        <v>23</v>
+        <v>22</v>
       </c>
       <c r="K19" s="0" t="n">
         <v>180</v>
@@ -956,7 +947,7 @@
         <v>17</v>
       </c>
       <c r="J20" s="0" t="s">
-        <v>24</v>
+        <v>23</v>
       </c>
       <c r="K20" s="0" t="n">
         <v>180</v>
@@ -991,7 +982,7 @@
         <v>17</v>
       </c>
       <c r="J21" s="0" t="s">
-        <v>25</v>
+        <v>24</v>
       </c>
       <c r="K21" s="0" t="n">
         <v>180</v>
@@ -1026,7 +1017,7 @@
         <v>17</v>
       </c>
       <c r="J22" s="0" t="s">
-        <v>20</v>
+        <v>19</v>
       </c>
       <c r="K22" s="0" t="n">
         <v>1440</v>
@@ -1061,7 +1052,7 @@
         <v>17</v>
       </c>
       <c r="J23" s="0" t="s">
-        <v>21</v>
+        <v>20</v>
       </c>
       <c r="K23" s="0" t="n">
         <v>1440</v>
@@ -1096,7 +1087,7 @@
         <v>17</v>
       </c>
       <c r="J24" s="0" t="s">
-        <v>22</v>
+        <v>21</v>
       </c>
       <c r="K24" s="0" t="n">
         <v>1440</v>
@@ -1131,7 +1122,7 @@
         <v>17</v>
       </c>
       <c r="J25" s="0" t="s">
-        <v>23</v>
+        <v>22</v>
       </c>
       <c r="K25" s="0" t="n">
         <v>1440</v>
@@ -1166,7 +1157,7 @@
         <v>17</v>
       </c>
       <c r="J26" s="0" t="s">
-        <v>24</v>
+        <v>23</v>
       </c>
       <c r="K26" s="0" t="n">
         <v>1440</v>
@@ -1201,7 +1192,7 @@
         <v>17</v>
       </c>
       <c r="J27" s="0" t="s">
-        <v>25</v>
+        <v>24</v>
       </c>
       <c r="K27" s="0" t="n">
         <v>1440</v>

</xml_diff>

<commit_message>
continuing major accuracy cleaning
</commit_message>
<xml_diff>
--- a/bioSample/bioSample_hbrown_01.16.20.xlsx
+++ b/bioSample/bioSample_hbrown_01.16.20.xlsx
@@ -20,7 +20,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="220" uniqueCount="25">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="220" uniqueCount="26">
   <si>
     <t xml:space="preserve">harvestDate</t>
   </si>
@@ -71,6 +71,9 @@
   </si>
   <si>
     <t xml:space="preserve">CNAG_00000</t>
+  </si>
+  <si>
+    <t xml:space="preserve">None</t>
   </si>
   <si>
     <t xml:space="preserve">NA</t>
@@ -214,7 +217,7 @@
   <dimension ref="A1:Z27"/>
   <sheetViews>
     <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="B4" activeCellId="0" sqref="B4"/>
+      <selection pane="topLeft" activeCell="H2" activeCellId="0" sqref="H2:H27"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="16" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
@@ -278,7 +281,7 @@
       <c r="Y1" s="2"/>
       <c r="Z1" s="2"/>
     </row>
-    <row r="2" customFormat="false" ht="16" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="2" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A2" s="0" t="s">
         <v>12</v>
       </c>
@@ -301,10 +304,10 @@
         <v>17</v>
       </c>
       <c r="I2" s="3" t="s">
-        <v>17</v>
+        <v>18</v>
       </c>
       <c r="J2" s="0" t="s">
-        <v>18</v>
+        <v>19</v>
       </c>
       <c r="K2" s="0" t="n">
         <v>0</v>
@@ -349,10 +352,10 @@
         <v>17</v>
       </c>
       <c r="I3" s="3" t="s">
-        <v>17</v>
+        <v>18</v>
       </c>
       <c r="J3" s="0" t="s">
-        <v>18</v>
+        <v>19</v>
       </c>
       <c r="K3" s="0" t="n">
         <v>0</v>
@@ -361,7 +364,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="4" customFormat="false" ht="16" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="4" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A4" s="0" t="s">
         <v>12</v>
       </c>
@@ -384,10 +387,10 @@
         <v>17</v>
       </c>
       <c r="I4" s="3" t="s">
-        <v>17</v>
+        <v>18</v>
       </c>
       <c r="J4" s="0" t="s">
-        <v>19</v>
+        <v>20</v>
       </c>
       <c r="K4" s="0" t="n">
         <v>30</v>
@@ -396,7 +399,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="5" customFormat="false" ht="16" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="5" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A5" s="0" t="s">
         <v>12</v>
       </c>
@@ -419,10 +422,10 @@
         <v>17</v>
       </c>
       <c r="I5" s="3" t="s">
-        <v>17</v>
+        <v>18</v>
       </c>
       <c r="J5" s="0" t="s">
-        <v>20</v>
+        <v>21</v>
       </c>
       <c r="K5" s="0" t="n">
         <v>30</v>
@@ -431,7 +434,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="6" customFormat="false" ht="16" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="6" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A6" s="0" t="s">
         <v>12</v>
       </c>
@@ -454,10 +457,10 @@
         <v>17</v>
       </c>
       <c r="I6" s="3" t="s">
-        <v>17</v>
+        <v>18</v>
       </c>
       <c r="J6" s="0" t="s">
-        <v>21</v>
+        <v>22</v>
       </c>
       <c r="K6" s="0" t="n">
         <v>30</v>
@@ -466,7 +469,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="7" customFormat="false" ht="16" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="7" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A7" s="0" t="s">
         <v>12</v>
       </c>
@@ -489,10 +492,10 @@
         <v>17</v>
       </c>
       <c r="I7" s="3" t="s">
-        <v>17</v>
+        <v>18</v>
       </c>
       <c r="J7" s="0" t="s">
-        <v>22</v>
+        <v>23</v>
       </c>
       <c r="K7" s="0" t="n">
         <v>30</v>
@@ -501,7 +504,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="8" customFormat="false" ht="16" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="8" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A8" s="0" t="s">
         <v>12</v>
       </c>
@@ -524,10 +527,10 @@
         <v>17</v>
       </c>
       <c r="I8" s="3" t="s">
-        <v>17</v>
+        <v>18</v>
       </c>
       <c r="J8" s="0" t="s">
-        <v>23</v>
+        <v>24</v>
       </c>
       <c r="K8" s="0" t="n">
         <v>30</v>
@@ -536,7 +539,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="9" customFormat="false" ht="16" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="9" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A9" s="0" t="s">
         <v>12</v>
       </c>
@@ -559,10 +562,10 @@
         <v>17</v>
       </c>
       <c r="I9" s="3" t="s">
-        <v>17</v>
+        <v>18</v>
       </c>
       <c r="J9" s="0" t="s">
-        <v>24</v>
+        <v>25</v>
       </c>
       <c r="K9" s="0" t="n">
         <v>30</v>
@@ -571,7 +574,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="10" customFormat="false" ht="16" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="10" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A10" s="0" t="s">
         <v>12</v>
       </c>
@@ -594,10 +597,10 @@
         <v>17</v>
       </c>
       <c r="I10" s="3" t="s">
-        <v>17</v>
+        <v>18</v>
       </c>
       <c r="J10" s="0" t="s">
-        <v>19</v>
+        <v>20</v>
       </c>
       <c r="K10" s="0" t="n">
         <v>90</v>
@@ -606,7 +609,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="11" customFormat="false" ht="16" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="11" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A11" s="0" t="s">
         <v>12</v>
       </c>
@@ -629,10 +632,10 @@
         <v>17</v>
       </c>
       <c r="I11" s="3" t="s">
-        <v>17</v>
+        <v>18</v>
       </c>
       <c r="J11" s="0" t="s">
-        <v>20</v>
+        <v>21</v>
       </c>
       <c r="K11" s="0" t="n">
         <v>90</v>
@@ -641,7 +644,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="12" customFormat="false" ht="16" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="12" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A12" s="0" t="s">
         <v>12</v>
       </c>
@@ -664,10 +667,10 @@
         <v>17</v>
       </c>
       <c r="I12" s="3" t="s">
-        <v>17</v>
+        <v>18</v>
       </c>
       <c r="J12" s="0" t="s">
-        <v>21</v>
+        <v>22</v>
       </c>
       <c r="K12" s="0" t="n">
         <v>90</v>
@@ -676,7 +679,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="13" customFormat="false" ht="16" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="13" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A13" s="0" t="s">
         <v>12</v>
       </c>
@@ -699,10 +702,10 @@
         <v>17</v>
       </c>
       <c r="I13" s="3" t="s">
-        <v>17</v>
+        <v>18</v>
       </c>
       <c r="J13" s="0" t="s">
-        <v>22</v>
+        <v>23</v>
       </c>
       <c r="K13" s="0" t="n">
         <v>90</v>
@@ -711,7 +714,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="14" customFormat="false" ht="16" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="14" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A14" s="0" t="s">
         <v>12</v>
       </c>
@@ -734,10 +737,10 @@
         <v>17</v>
       </c>
       <c r="I14" s="3" t="s">
-        <v>17</v>
+        <v>18</v>
       </c>
       <c r="J14" s="0" t="s">
-        <v>23</v>
+        <v>24</v>
       </c>
       <c r="K14" s="0" t="n">
         <v>90</v>
@@ -746,7 +749,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="15" customFormat="false" ht="16" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="15" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A15" s="0" t="s">
         <v>12</v>
       </c>
@@ -769,10 +772,10 @@
         <v>17</v>
       </c>
       <c r="I15" s="3" t="s">
-        <v>17</v>
+        <v>18</v>
       </c>
       <c r="J15" s="0" t="s">
-        <v>24</v>
+        <v>25</v>
       </c>
       <c r="K15" s="0" t="n">
         <v>90</v>
@@ -781,7 +784,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="16" customFormat="false" ht="16" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="16" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A16" s="0" t="s">
         <v>12</v>
       </c>
@@ -804,10 +807,10 @@
         <v>17</v>
       </c>
       <c r="I16" s="3" t="s">
-        <v>17</v>
+        <v>18</v>
       </c>
       <c r="J16" s="0" t="s">
-        <v>19</v>
+        <v>20</v>
       </c>
       <c r="K16" s="0" t="n">
         <v>180</v>
@@ -816,7 +819,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="17" customFormat="false" ht="16" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="17" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A17" s="0" t="s">
         <v>12</v>
       </c>
@@ -839,10 +842,10 @@
         <v>17</v>
       </c>
       <c r="I17" s="3" t="s">
-        <v>17</v>
+        <v>18</v>
       </c>
       <c r="J17" s="0" t="s">
-        <v>20</v>
+        <v>21</v>
       </c>
       <c r="K17" s="0" t="n">
         <v>180</v>
@@ -851,7 +854,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="18" customFormat="false" ht="16" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="18" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A18" s="0" t="s">
         <v>12</v>
       </c>
@@ -874,10 +877,10 @@
         <v>17</v>
       </c>
       <c r="I18" s="3" t="s">
-        <v>17</v>
+        <v>18</v>
       </c>
       <c r="J18" s="0" t="s">
-        <v>21</v>
+        <v>22</v>
       </c>
       <c r="K18" s="0" t="n">
         <v>180</v>
@@ -886,7 +889,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="19" customFormat="false" ht="16" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="19" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A19" s="0" t="s">
         <v>12</v>
       </c>
@@ -909,10 +912,10 @@
         <v>17</v>
       </c>
       <c r="I19" s="3" t="s">
-        <v>17</v>
+        <v>18</v>
       </c>
       <c r="J19" s="0" t="s">
-        <v>22</v>
+        <v>23</v>
       </c>
       <c r="K19" s="0" t="n">
         <v>180</v>
@@ -921,7 +924,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="20" customFormat="false" ht="16" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="20" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A20" s="0" t="s">
         <v>12</v>
       </c>
@@ -944,10 +947,10 @@
         <v>17</v>
       </c>
       <c r="I20" s="3" t="s">
-        <v>17</v>
+        <v>18</v>
       </c>
       <c r="J20" s="0" t="s">
-        <v>23</v>
+        <v>24</v>
       </c>
       <c r="K20" s="0" t="n">
         <v>180</v>
@@ -956,7 +959,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="21" customFormat="false" ht="16" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="21" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A21" s="0" t="s">
         <v>12</v>
       </c>
@@ -979,10 +982,10 @@
         <v>17</v>
       </c>
       <c r="I21" s="3" t="s">
-        <v>17</v>
+        <v>18</v>
       </c>
       <c r="J21" s="0" t="s">
-        <v>24</v>
+        <v>25</v>
       </c>
       <c r="K21" s="0" t="n">
         <v>180</v>
@@ -991,7 +994,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="22" customFormat="false" ht="16" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="22" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A22" s="0" t="s">
         <v>12</v>
       </c>
@@ -1014,10 +1017,10 @@
         <v>17</v>
       </c>
       <c r="I22" s="3" t="s">
-        <v>17</v>
+        <v>18</v>
       </c>
       <c r="J22" s="0" t="s">
-        <v>19</v>
+        <v>20</v>
       </c>
       <c r="K22" s="0" t="n">
         <v>1440</v>
@@ -1026,7 +1029,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="23" customFormat="false" ht="16" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="23" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A23" s="0" t="s">
         <v>12</v>
       </c>
@@ -1049,10 +1052,10 @@
         <v>17</v>
       </c>
       <c r="I23" s="3" t="s">
-        <v>17</v>
+        <v>18</v>
       </c>
       <c r="J23" s="0" t="s">
-        <v>20</v>
+        <v>21</v>
       </c>
       <c r="K23" s="0" t="n">
         <v>1440</v>
@@ -1061,7 +1064,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="24" customFormat="false" ht="16" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="24" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A24" s="0" t="s">
         <v>12</v>
       </c>
@@ -1084,10 +1087,10 @@
         <v>17</v>
       </c>
       <c r="I24" s="3" t="s">
-        <v>17</v>
+        <v>18</v>
       </c>
       <c r="J24" s="0" t="s">
-        <v>21</v>
+        <v>22</v>
       </c>
       <c r="K24" s="0" t="n">
         <v>1440</v>
@@ -1096,7 +1099,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="25" customFormat="false" ht="16" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="25" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A25" s="0" t="s">
         <v>12</v>
       </c>
@@ -1119,10 +1122,10 @@
         <v>17</v>
       </c>
       <c r="I25" s="3" t="s">
-        <v>17</v>
+        <v>18</v>
       </c>
       <c r="J25" s="0" t="s">
-        <v>22</v>
+        <v>23</v>
       </c>
       <c r="K25" s="0" t="n">
         <v>1440</v>
@@ -1131,7 +1134,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="26" customFormat="false" ht="16" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="26" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A26" s="0" t="s">
         <v>12</v>
       </c>
@@ -1154,10 +1157,10 @@
         <v>17</v>
       </c>
       <c r="I26" s="3" t="s">
-        <v>17</v>
+        <v>18</v>
       </c>
       <c r="J26" s="0" t="s">
-        <v>23</v>
+        <v>24</v>
       </c>
       <c r="K26" s="0" t="n">
         <v>1440</v>
@@ -1166,7 +1169,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="27" customFormat="false" ht="16" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="27" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A27" s="0" t="s">
         <v>12</v>
       </c>
@@ -1189,10 +1192,10 @@
         <v>17</v>
       </c>
       <c r="I27" s="3" t="s">
-        <v>17</v>
+        <v>18</v>
       </c>
       <c r="J27" s="0" t="s">
-        <v>24</v>
+        <v>25</v>
       </c>
       <c r="K27" s="0" t="n">
         <v>1440</v>

</xml_diff>

<commit_message>
updating files to conform to standard
</commit_message>
<xml_diff>
--- a/bioSample/bioSample_hbrown_01.16.20.xlsx
+++ b/bioSample/bioSample_hbrown_01.16.20.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/hollybrown/database_files/bioSample/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{A4AD4CEB-DBD6-384D-844C-836AC3A8B8B7}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{6F71123B-57D5-2342-8BCC-C4FE77C64DE6}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="6120" windowWidth="16380" windowHeight="8200" tabRatio="500" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="0" yWindow="6120" windowWidth="23420" windowHeight="8200" tabRatio="500" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -25,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="166" uniqueCount="22">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="165" uniqueCount="21">
   <si>
     <t>harvestDate</t>
   </si>
@@ -37,9 +37,6 @@
   </si>
   <si>
     <t>experimentDesign</t>
-  </si>
-  <si>
-    <t>experimentObservations</t>
   </si>
   <si>
     <t>strain</t>
@@ -133,13 +130,10 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="4">
+  <cellXfs count="3">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment horizontal="right"/>
-    </xf>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -454,10 +448,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:Z27"/>
+  <dimension ref="A1:W27"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="C1" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="J29" sqref="J29"/>
+    <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="E1" sqref="E1:E1048576"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -466,10 +460,10 @@
     <col min="2" max="2" width="16.1640625" customWidth="1"/>
     <col min="3" max="3" width="10.6640625" customWidth="1"/>
     <col min="4" max="4" width="14" customWidth="1"/>
-    <col min="5" max="1025" width="10.6640625" customWidth="1"/>
+    <col min="5" max="1022" width="10.6640625" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:26" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="1" spans="1:23" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A1" t="s">
         <v>0</v>
       </c>
@@ -491,15 +485,15 @@
       <c r="G1" t="s">
         <v>6</v>
       </c>
-      <c r="J1" t="s">
+      <c r="H1" t="s">
         <v>7</v>
       </c>
-      <c r="K1" t="s">
+      <c r="I1" t="s">
         <v>8</v>
       </c>
-      <c r="L1" t="s">
-        <v>9</v>
-      </c>
+      <c r="J1" s="2"/>
+      <c r="K1" s="2"/>
+      <c r="L1" s="2"/>
       <c r="M1" s="2"/>
       <c r="N1" s="2"/>
       <c r="O1" s="2"/>
@@ -511,21 +505,21 @@
       <c r="U1" s="2"/>
       <c r="V1" s="2"/>
       <c r="W1" s="2"/>
-      <c r="X1" s="2"/>
-      <c r="Y1" s="2"/>
-      <c r="Z1" s="2"/>
-    </row>
-    <row r="2" spans="1:26" x14ac:dyDescent="0.2">
+    </row>
+    <row r="2" spans="1:23" x14ac:dyDescent="0.2">
       <c r="A2" t="s">
-        <v>10</v>
+        <v>9</v>
       </c>
       <c r="B2" t="s">
-        <v>11</v>
+        <v>10</v>
       </c>
       <c r="C2">
         <v>1</v>
       </c>
       <c r="D2" s="2" t="s">
+        <v>11</v>
+      </c>
+      <c r="E2" t="s">
         <v>12</v>
       </c>
       <c r="F2" t="s">
@@ -534,17 +528,15 @@
       <c r="G2" t="s">
         <v>14</v>
       </c>
-      <c r="H2" s="2"/>
-      <c r="I2" s="3"/>
-      <c r="J2" t="s">
-        <v>15</v>
-      </c>
-      <c r="K2">
+      <c r="H2">
         <v>0</v>
       </c>
-      <c r="L2">
-        <v>1</v>
-      </c>
+      <c r="I2">
+        <v>1</v>
+      </c>
+      <c r="K2" s="2"/>
+      <c r="L2" s="2"/>
+      <c r="M2" s="2"/>
       <c r="N2" s="2"/>
       <c r="O2" s="2"/>
       <c r="P2" s="2"/>
@@ -555,21 +547,21 @@
       <c r="U2" s="2"/>
       <c r="V2" s="2"/>
       <c r="W2" s="2"/>
-      <c r="X2" s="2"/>
-      <c r="Y2" s="2"/>
-      <c r="Z2" s="2"/>
-    </row>
-    <row r="3" spans="1:26" x14ac:dyDescent="0.2">
+    </row>
+    <row r="3" spans="1:23" x14ac:dyDescent="0.2">
       <c r="A3" t="s">
-        <v>10</v>
+        <v>9</v>
       </c>
       <c r="B3" t="s">
-        <v>11</v>
+        <v>10</v>
       </c>
       <c r="C3">
         <v>2</v>
       </c>
       <c r="D3" s="2" t="s">
+        <v>11</v>
+      </c>
+      <c r="E3" t="s">
         <v>12</v>
       </c>
       <c r="F3" t="s">
@@ -578,759 +570,706 @@
       <c r="G3" t="s">
         <v>14</v>
       </c>
-      <c r="H3" s="2"/>
-      <c r="I3" s="3"/>
-      <c r="J3" t="s">
-        <v>15</v>
-      </c>
-      <c r="K3">
+      <c r="H3">
         <v>0</v>
       </c>
-      <c r="L3">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="4" spans="1:26" x14ac:dyDescent="0.2">
+      <c r="I3">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="4" spans="1:23" x14ac:dyDescent="0.2">
       <c r="A4" t="s">
-        <v>10</v>
+        <v>9</v>
       </c>
       <c r="B4" t="s">
-        <v>11</v>
+        <v>10</v>
       </c>
       <c r="C4">
         <v>3</v>
       </c>
       <c r="D4" s="2" t="s">
+        <v>11</v>
+      </c>
+      <c r="E4" t="s">
         <v>12</v>
       </c>
       <c r="F4" t="s">
         <v>13</v>
       </c>
       <c r="G4" t="s">
-        <v>14</v>
-      </c>
-      <c r="H4" s="2"/>
-      <c r="I4" s="3"/>
-      <c r="J4" t="s">
-        <v>16</v>
-      </c>
-      <c r="K4">
+        <v>15</v>
+      </c>
+      <c r="H4">
         <v>30</v>
       </c>
-      <c r="L4">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="5" spans="1:26" x14ac:dyDescent="0.2">
+      <c r="I4">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="5" spans="1:23" x14ac:dyDescent="0.2">
       <c r="A5" t="s">
-        <v>10</v>
+        <v>9</v>
       </c>
       <c r="B5" t="s">
-        <v>11</v>
+        <v>10</v>
       </c>
       <c r="C5">
         <v>4</v>
       </c>
       <c r="D5" s="2" t="s">
+        <v>11</v>
+      </c>
+      <c r="E5" t="s">
         <v>12</v>
       </c>
       <c r="F5" t="s">
         <v>13</v>
       </c>
       <c r="G5" t="s">
-        <v>14</v>
-      </c>
-      <c r="H5" s="2"/>
-      <c r="I5" s="3"/>
-      <c r="J5" t="s">
-        <v>17</v>
-      </c>
-      <c r="K5">
+        <v>16</v>
+      </c>
+      <c r="H5">
         <v>30</v>
       </c>
-      <c r="L5">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="6" spans="1:26" x14ac:dyDescent="0.2">
+      <c r="I5">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="6" spans="1:23" x14ac:dyDescent="0.2">
       <c r="A6" t="s">
-        <v>10</v>
+        <v>9</v>
       </c>
       <c r="B6" t="s">
-        <v>11</v>
+        <v>10</v>
       </c>
       <c r="C6">
         <v>5</v>
       </c>
       <c r="D6" s="2" t="s">
+        <v>11</v>
+      </c>
+      <c r="E6" t="s">
         <v>12</v>
       </c>
       <c r="F6" t="s">
         <v>13</v>
       </c>
       <c r="G6" t="s">
-        <v>14</v>
-      </c>
-      <c r="H6" s="2"/>
-      <c r="I6" s="3"/>
-      <c r="J6" t="s">
-        <v>18</v>
-      </c>
-      <c r="K6">
+        <v>17</v>
+      </c>
+      <c r="H6">
         <v>30</v>
       </c>
-      <c r="L6">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="7" spans="1:26" x14ac:dyDescent="0.2">
+      <c r="I6">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="7" spans="1:23" x14ac:dyDescent="0.2">
       <c r="A7" t="s">
-        <v>10</v>
+        <v>9</v>
       </c>
       <c r="B7" t="s">
-        <v>11</v>
+        <v>10</v>
       </c>
       <c r="C7">
         <v>6</v>
       </c>
       <c r="D7" s="2" t="s">
+        <v>11</v>
+      </c>
+      <c r="E7" t="s">
         <v>12</v>
       </c>
       <c r="F7" t="s">
         <v>13</v>
       </c>
       <c r="G7" t="s">
-        <v>14</v>
-      </c>
-      <c r="H7" s="2"/>
-      <c r="I7" s="3"/>
-      <c r="J7" t="s">
-        <v>19</v>
-      </c>
-      <c r="K7">
+        <v>18</v>
+      </c>
+      <c r="H7">
         <v>30</v>
       </c>
-      <c r="L7">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="8" spans="1:26" x14ac:dyDescent="0.2">
+      <c r="I7">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="8" spans="1:23" x14ac:dyDescent="0.2">
       <c r="A8" t="s">
-        <v>10</v>
+        <v>9</v>
       </c>
       <c r="B8" t="s">
-        <v>11</v>
+        <v>10</v>
       </c>
       <c r="C8">
         <v>7</v>
       </c>
       <c r="D8" s="2" t="s">
+        <v>11</v>
+      </c>
+      <c r="E8" t="s">
         <v>12</v>
       </c>
       <c r="F8" t="s">
         <v>13</v>
       </c>
       <c r="G8" t="s">
-        <v>14</v>
-      </c>
-      <c r="H8" s="2"/>
-      <c r="I8" s="3"/>
-      <c r="J8" t="s">
-        <v>20</v>
-      </c>
-      <c r="K8">
+        <v>19</v>
+      </c>
+      <c r="H8">
         <v>30</v>
       </c>
-      <c r="L8">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="9" spans="1:26" x14ac:dyDescent="0.2">
+      <c r="I8">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="9" spans="1:23" x14ac:dyDescent="0.2">
       <c r="A9" t="s">
-        <v>10</v>
+        <v>9</v>
       </c>
       <c r="B9" t="s">
-        <v>11</v>
+        <v>10</v>
       </c>
       <c r="C9">
         <v>8</v>
       </c>
       <c r="D9" s="2" t="s">
+        <v>11</v>
+      </c>
+      <c r="E9" t="s">
         <v>12</v>
       </c>
       <c r="F9" t="s">
         <v>13</v>
       </c>
       <c r="G9" t="s">
-        <v>14</v>
-      </c>
-      <c r="H9" s="2"/>
-      <c r="I9" s="3"/>
-      <c r="J9" t="s">
-        <v>21</v>
-      </c>
-      <c r="K9">
+        <v>20</v>
+      </c>
+      <c r="H9">
         <v>30</v>
       </c>
-      <c r="L9">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="10" spans="1:26" x14ac:dyDescent="0.2">
+      <c r="I9">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="10" spans="1:23" x14ac:dyDescent="0.2">
       <c r="A10" t="s">
-        <v>10</v>
+        <v>9</v>
       </c>
       <c r="B10" t="s">
-        <v>11</v>
+        <v>10</v>
       </c>
       <c r="C10">
         <v>9</v>
       </c>
       <c r="D10" s="2" t="s">
+        <v>11</v>
+      </c>
+      <c r="E10" t="s">
         <v>12</v>
       </c>
       <c r="F10" t="s">
         <v>13</v>
       </c>
       <c r="G10" t="s">
-        <v>14</v>
-      </c>
-      <c r="H10" s="2"/>
-      <c r="I10" s="3"/>
-      <c r="J10" t="s">
+        <v>15</v>
+      </c>
+      <c r="H10">
+        <v>90</v>
+      </c>
+      <c r="I10">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="11" spans="1:23" x14ac:dyDescent="0.2">
+      <c r="A11" t="s">
+        <v>9</v>
+      </c>
+      <c r="B11" t="s">
+        <v>10</v>
+      </c>
+      <c r="C11">
+        <v>10</v>
+      </c>
+      <c r="D11" s="2" t="s">
+        <v>11</v>
+      </c>
+      <c r="E11" t="s">
+        <v>12</v>
+      </c>
+      <c r="F11" t="s">
+        <v>13</v>
+      </c>
+      <c r="G11" t="s">
         <v>16</v>
       </c>
-      <c r="K10">
+      <c r="H11">
         <v>90</v>
       </c>
-      <c r="L10">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="11" spans="1:26" x14ac:dyDescent="0.2">
-      <c r="A11" t="s">
-        <v>10</v>
-      </c>
-      <c r="B11" t="s">
-        <v>11</v>
-      </c>
-      <c r="C11">
-        <v>10</v>
-      </c>
-      <c r="D11" s="2" t="s">
-        <v>12</v>
-      </c>
-      <c r="F11" t="s">
-        <v>13</v>
-      </c>
-      <c r="G11" t="s">
-        <v>14</v>
-      </c>
-      <c r="H11" s="2"/>
-      <c r="I11" s="3"/>
-      <c r="J11" t="s">
+      <c r="I11">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="12" spans="1:23" x14ac:dyDescent="0.2">
+      <c r="A12" t="s">
+        <v>9</v>
+      </c>
+      <c r="B12" t="s">
+        <v>10</v>
+      </c>
+      <c r="C12">
+        <v>11</v>
+      </c>
+      <c r="D12" s="2" t="s">
+        <v>11</v>
+      </c>
+      <c r="E12" t="s">
+        <v>12</v>
+      </c>
+      <c r="F12" t="s">
+        <v>13</v>
+      </c>
+      <c r="G12" t="s">
         <v>17</v>
       </c>
-      <c r="K11">
+      <c r="H12">
         <v>90</v>
       </c>
-      <c r="L11">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="12" spans="1:26" x14ac:dyDescent="0.2">
-      <c r="A12" t="s">
-        <v>10</v>
-      </c>
-      <c r="B12" t="s">
-        <v>11</v>
-      </c>
-      <c r="C12">
-        <v>11</v>
-      </c>
-      <c r="D12" s="2" t="s">
-        <v>12</v>
-      </c>
-      <c r="F12" t="s">
-        <v>13</v>
-      </c>
-      <c r="G12" t="s">
-        <v>14</v>
-      </c>
-      <c r="H12" s="2"/>
-      <c r="I12" s="3"/>
-      <c r="J12" t="s">
+      <c r="I12">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="13" spans="1:23" x14ac:dyDescent="0.2">
+      <c r="A13" t="s">
+        <v>9</v>
+      </c>
+      <c r="B13" t="s">
+        <v>10</v>
+      </c>
+      <c r="C13">
+        <v>12</v>
+      </c>
+      <c r="D13" s="2" t="s">
+        <v>11</v>
+      </c>
+      <c r="E13" t="s">
+        <v>12</v>
+      </c>
+      <c r="F13" t="s">
+        <v>13</v>
+      </c>
+      <c r="G13" t="s">
         <v>18</v>
       </c>
-      <c r="K12">
+      <c r="H13">
         <v>90</v>
       </c>
-      <c r="L12">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="13" spans="1:26" x14ac:dyDescent="0.2">
-      <c r="A13" t="s">
-        <v>10</v>
-      </c>
-      <c r="B13" t="s">
-        <v>11</v>
-      </c>
-      <c r="C13">
-        <v>12</v>
-      </c>
-      <c r="D13" s="2" t="s">
-        <v>12</v>
-      </c>
-      <c r="F13" t="s">
-        <v>13</v>
-      </c>
-      <c r="G13" t="s">
-        <v>14</v>
-      </c>
-      <c r="H13" s="2"/>
-      <c r="I13" s="3"/>
-      <c r="J13" t="s">
+      <c r="I13">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="14" spans="1:23" x14ac:dyDescent="0.2">
+      <c r="A14" t="s">
+        <v>9</v>
+      </c>
+      <c r="B14" t="s">
+        <v>10</v>
+      </c>
+      <c r="C14">
+        <v>13</v>
+      </c>
+      <c r="D14" s="2" t="s">
+        <v>11</v>
+      </c>
+      <c r="E14" t="s">
+        <v>12</v>
+      </c>
+      <c r="F14" t="s">
+        <v>13</v>
+      </c>
+      <c r="G14" t="s">
         <v>19</v>
       </c>
-      <c r="K13">
+      <c r="H14">
         <v>90</v>
       </c>
-      <c r="L13">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="14" spans="1:26" x14ac:dyDescent="0.2">
-      <c r="A14" t="s">
-        <v>10</v>
-      </c>
-      <c r="B14" t="s">
-        <v>11</v>
-      </c>
-      <c r="C14">
-        <v>13</v>
-      </c>
-      <c r="D14" s="2" t="s">
-        <v>12</v>
-      </c>
-      <c r="F14" t="s">
-        <v>13</v>
-      </c>
-      <c r="G14" t="s">
-        <v>14</v>
-      </c>
-      <c r="H14" s="2"/>
-      <c r="I14" s="3"/>
-      <c r="J14" t="s">
-        <v>20</v>
-      </c>
-      <c r="K14">
-        <v>90</v>
-      </c>
-      <c r="L14">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="15" spans="1:26" x14ac:dyDescent="0.2">
+      <c r="I14">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="15" spans="1:23" x14ac:dyDescent="0.2">
       <c r="A15" t="s">
-        <v>10</v>
+        <v>9</v>
       </c>
       <c r="B15" t="s">
-        <v>11</v>
+        <v>10</v>
       </c>
       <c r="C15">
         <v>14</v>
       </c>
       <c r="D15" s="2" t="s">
+        <v>11</v>
+      </c>
+      <c r="E15" t="s">
         <v>12</v>
       </c>
       <c r="F15" t="s">
         <v>13</v>
       </c>
       <c r="G15" t="s">
-        <v>14</v>
-      </c>
-      <c r="H15" s="2"/>
-      <c r="I15" s="3"/>
-      <c r="J15" t="s">
-        <v>21</v>
-      </c>
-      <c r="K15">
+        <v>20</v>
+      </c>
+      <c r="H15">
         <v>90</v>
       </c>
-      <c r="L15">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="16" spans="1:26" x14ac:dyDescent="0.2">
+      <c r="I15">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="16" spans="1:23" x14ac:dyDescent="0.2">
       <c r="A16" t="s">
-        <v>10</v>
+        <v>9</v>
       </c>
       <c r="B16" t="s">
-        <v>11</v>
+        <v>10</v>
       </c>
       <c r="C16">
         <v>15</v>
       </c>
       <c r="D16" s="2" t="s">
+        <v>11</v>
+      </c>
+      <c r="E16" t="s">
         <v>12</v>
       </c>
       <c r="F16" t="s">
         <v>13</v>
       </c>
       <c r="G16" t="s">
-        <v>14</v>
-      </c>
-      <c r="H16" s="2"/>
-      <c r="I16" s="3"/>
-      <c r="J16" t="s">
-        <v>16</v>
-      </c>
-      <c r="K16">
+        <v>15</v>
+      </c>
+      <c r="H16">
         <v>180</v>
       </c>
-      <c r="L16">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="17" spans="1:12" x14ac:dyDescent="0.2">
+      <c r="I16">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="17" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A17" t="s">
-        <v>10</v>
+        <v>9</v>
       </c>
       <c r="B17" t="s">
-        <v>11</v>
+        <v>10</v>
       </c>
       <c r="C17">
         <v>16</v>
       </c>
       <c r="D17" s="2" t="s">
+        <v>11</v>
+      </c>
+      <c r="E17" t="s">
         <v>12</v>
       </c>
       <c r="F17" t="s">
         <v>13</v>
       </c>
       <c r="G17" t="s">
-        <v>14</v>
-      </c>
-      <c r="H17" s="2"/>
-      <c r="I17" s="3"/>
-      <c r="J17" t="s">
-        <v>17</v>
-      </c>
-      <c r="K17">
+        <v>16</v>
+      </c>
+      <c r="H17">
         <v>180</v>
       </c>
-      <c r="L17">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="18" spans="1:12" x14ac:dyDescent="0.2">
+      <c r="I17">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="18" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A18" t="s">
-        <v>10</v>
+        <v>9</v>
       </c>
       <c r="B18" t="s">
-        <v>11</v>
+        <v>10</v>
       </c>
       <c r="C18">
         <v>17</v>
       </c>
       <c r="D18" s="2" t="s">
+        <v>11</v>
+      </c>
+      <c r="E18" t="s">
         <v>12</v>
       </c>
       <c r="F18" t="s">
         <v>13</v>
       </c>
       <c r="G18" t="s">
-        <v>14</v>
-      </c>
-      <c r="H18" s="2"/>
-      <c r="I18" s="3"/>
-      <c r="J18" t="s">
-        <v>18</v>
-      </c>
-      <c r="K18">
+        <v>17</v>
+      </c>
+      <c r="H18">
         <v>180</v>
       </c>
-      <c r="L18">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="19" spans="1:12" x14ac:dyDescent="0.2">
+      <c r="I18">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="19" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A19" t="s">
-        <v>10</v>
+        <v>9</v>
       </c>
       <c r="B19" t="s">
-        <v>11</v>
+        <v>10</v>
       </c>
       <c r="C19">
         <v>18</v>
       </c>
       <c r="D19" s="2" t="s">
+        <v>11</v>
+      </c>
+      <c r="E19" t="s">
         <v>12</v>
       </c>
       <c r="F19" t="s">
         <v>13</v>
       </c>
       <c r="G19" t="s">
-        <v>14</v>
-      </c>
-      <c r="H19" s="2"/>
-      <c r="I19" s="3"/>
-      <c r="J19" t="s">
-        <v>19</v>
-      </c>
-      <c r="K19">
+        <v>18</v>
+      </c>
+      <c r="H19">
         <v>180</v>
       </c>
-      <c r="L19">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="20" spans="1:12" x14ac:dyDescent="0.2">
+      <c r="I19">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="20" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A20" t="s">
-        <v>10</v>
+        <v>9</v>
       </c>
       <c r="B20" t="s">
-        <v>11</v>
+        <v>10</v>
       </c>
       <c r="C20">
         <v>19</v>
       </c>
       <c r="D20" s="2" t="s">
+        <v>11</v>
+      </c>
+      <c r="E20" t="s">
         <v>12</v>
       </c>
       <c r="F20" t="s">
         <v>13</v>
       </c>
       <c r="G20" t="s">
-        <v>14</v>
-      </c>
-      <c r="H20" s="2"/>
-      <c r="I20" s="3"/>
-      <c r="J20" t="s">
-        <v>20</v>
-      </c>
-      <c r="K20">
+        <v>19</v>
+      </c>
+      <c r="H20">
         <v>180</v>
       </c>
-      <c r="L20">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="21" spans="1:12" x14ac:dyDescent="0.2">
+      <c r="I20">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="21" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A21" t="s">
-        <v>10</v>
+        <v>9</v>
       </c>
       <c r="B21" t="s">
-        <v>11</v>
+        <v>10</v>
       </c>
       <c r="C21">
         <v>20</v>
       </c>
       <c r="D21" s="2" t="s">
+        <v>11</v>
+      </c>
+      <c r="E21" t="s">
         <v>12</v>
       </c>
       <c r="F21" t="s">
         <v>13</v>
       </c>
       <c r="G21" t="s">
-        <v>14</v>
-      </c>
-      <c r="H21" s="2"/>
-      <c r="I21" s="3"/>
-      <c r="J21" t="s">
-        <v>21</v>
-      </c>
-      <c r="K21">
+        <v>20</v>
+      </c>
+      <c r="H21">
         <v>180</v>
       </c>
-      <c r="L21">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="22" spans="1:12" x14ac:dyDescent="0.2">
+      <c r="I21">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="22" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A22" t="s">
-        <v>10</v>
+        <v>9</v>
       </c>
       <c r="B22" t="s">
-        <v>11</v>
+        <v>10</v>
       </c>
       <c r="C22">
         <v>21</v>
       </c>
       <c r="D22" s="2" t="s">
+        <v>11</v>
+      </c>
+      <c r="E22" t="s">
         <v>12</v>
       </c>
       <c r="F22" t="s">
         <v>13</v>
       </c>
       <c r="G22" t="s">
-        <v>14</v>
-      </c>
-      <c r="H22" s="2"/>
-      <c r="I22" s="3"/>
-      <c r="J22" t="s">
-        <v>16</v>
-      </c>
-      <c r="K22">
+        <v>15</v>
+      </c>
+      <c r="H22">
         <v>1440</v>
       </c>
-      <c r="L22">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="23" spans="1:12" x14ac:dyDescent="0.2">
+      <c r="I22">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="23" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A23" t="s">
-        <v>10</v>
+        <v>9</v>
       </c>
       <c r="B23" t="s">
-        <v>11</v>
+        <v>10</v>
       </c>
       <c r="C23">
         <v>22</v>
       </c>
       <c r="D23" s="2" t="s">
+        <v>11</v>
+      </c>
+      <c r="E23" t="s">
         <v>12</v>
       </c>
       <c r="F23" t="s">
         <v>13</v>
       </c>
       <c r="G23" t="s">
-        <v>14</v>
-      </c>
-      <c r="H23" s="2"/>
-      <c r="I23" s="3"/>
-      <c r="J23" t="s">
-        <v>17</v>
-      </c>
-      <c r="K23">
+        <v>16</v>
+      </c>
+      <c r="H23">
         <v>1440</v>
       </c>
-      <c r="L23">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="24" spans="1:12" x14ac:dyDescent="0.2">
+      <c r="I23">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="24" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A24" t="s">
-        <v>10</v>
+        <v>9</v>
       </c>
       <c r="B24" t="s">
-        <v>11</v>
+        <v>10</v>
       </c>
       <c r="C24">
         <v>23</v>
       </c>
       <c r="D24" s="2" t="s">
+        <v>11</v>
+      </c>
+      <c r="E24" t="s">
         <v>12</v>
       </c>
       <c r="F24" t="s">
         <v>13</v>
       </c>
       <c r="G24" t="s">
-        <v>14</v>
-      </c>
-      <c r="H24" s="2"/>
-      <c r="I24" s="3"/>
-      <c r="J24" t="s">
-        <v>18</v>
-      </c>
-      <c r="K24">
+        <v>17</v>
+      </c>
+      <c r="H24">
         <v>1440</v>
       </c>
-      <c r="L24">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="25" spans="1:12" x14ac:dyDescent="0.2">
+      <c r="I24">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="25" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A25" t="s">
-        <v>10</v>
+        <v>9</v>
       </c>
       <c r="B25" t="s">
-        <v>11</v>
+        <v>10</v>
       </c>
       <c r="C25">
         <v>24</v>
       </c>
       <c r="D25" s="2" t="s">
+        <v>11</v>
+      </c>
+      <c r="E25" t="s">
         <v>12</v>
       </c>
       <c r="F25" t="s">
         <v>13</v>
       </c>
       <c r="G25" t="s">
-        <v>14</v>
-      </c>
-      <c r="H25" s="2"/>
-      <c r="I25" s="3"/>
-      <c r="J25" t="s">
-        <v>19</v>
-      </c>
-      <c r="K25">
+        <v>18</v>
+      </c>
+      <c r="H25">
         <v>1440</v>
       </c>
-      <c r="L25">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="26" spans="1:12" x14ac:dyDescent="0.2">
+      <c r="I25">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="26" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A26" t="s">
-        <v>10</v>
+        <v>9</v>
       </c>
       <c r="B26" t="s">
-        <v>11</v>
+        <v>10</v>
       </c>
       <c r="C26">
         <v>25</v>
       </c>
       <c r="D26" s="2" t="s">
+        <v>11</v>
+      </c>
+      <c r="E26" t="s">
         <v>12</v>
       </c>
       <c r="F26" t="s">
         <v>13</v>
       </c>
       <c r="G26" t="s">
-        <v>14</v>
-      </c>
-      <c r="H26" s="2"/>
-      <c r="I26" s="3"/>
-      <c r="J26" t="s">
-        <v>20</v>
-      </c>
-      <c r="K26">
+        <v>19</v>
+      </c>
+      <c r="H26">
         <v>1440</v>
       </c>
-      <c r="L26">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="27" spans="1:12" x14ac:dyDescent="0.2">
+      <c r="I26">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="27" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A27" t="s">
-        <v>10</v>
+        <v>9</v>
       </c>
       <c r="B27" t="s">
-        <v>11</v>
+        <v>10</v>
       </c>
       <c r="C27">
         <v>26</v>
       </c>
       <c r="D27" s="2" t="s">
+        <v>11</v>
+      </c>
+      <c r="E27" t="s">
         <v>12</v>
       </c>
       <c r="F27" t="s">
         <v>13</v>
       </c>
       <c r="G27" t="s">
-        <v>14</v>
-      </c>
-      <c r="H27" s="2"/>
-      <c r="I27" s="3"/>
-      <c r="J27" t="s">
-        <v>21</v>
-      </c>
-      <c r="K27">
+        <v>20</v>
+      </c>
+      <c r="H27">
         <v>1440</v>
       </c>
-      <c r="L27">
+      <c r="I27">
         <v>1</v>
       </c>
     </row>

</xml_diff>